<commit_message>
Updated ESPixel BOM with enclosure and glands
</commit_message>
<xml_diff>
--- a/ESPixelBOM.xlsx
+++ b/ESPixelBOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Description</t>
   </si>
@@ -90,9 +90,6 @@
     <t>WIFI</t>
   </si>
   <si>
-    <t>Spark</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -124,6 +121,27 @@
   </si>
   <si>
     <t>1212-1231-ND</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>HM1102-ND</t>
+  </si>
+  <si>
+    <t>Gland</t>
+  </si>
+  <si>
+    <t>7489K12</t>
+  </si>
+  <si>
+    <t>Mcmaster-carr</t>
+  </si>
+  <si>
+    <t>7807K31</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
   </si>
 </sst>
 </file>
@@ -166,12 +184,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -187,12 +211,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -498,7 +525,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:I11"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,10 +597,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -602,7 +629,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -643,24 +670,24 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F4:F22" si="2">E5*D5</f>
+        <f t="shared" ref="F5:F22" si="2">E5*D5</f>
         <v>0.28999999999999998</v>
       </c>
       <c r="G5">
         <v>0.12089999999999999</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H4:H23" si="3">G5*100*D5</f>
+        <f t="shared" ref="H5:H23" si="3">G5*100*D5</f>
         <v>12.09</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -688,7 +715,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -769,10 +796,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -797,10 +824,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -812,6 +839,7 @@
         <v>0.8</v>
       </c>
       <c r="F11">
+        <f t="shared" ref="F11:F14" si="4">E11*D11</f>
         <v>0.8</v>
       </c>
       <c r="G11">
@@ -819,6 +847,69 @@
       </c>
       <c r="H11">
         <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>6.47</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>3.74</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>3.74</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -882,7 +973,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -940,7 +1031,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -949,7 +1040,7 @@
       </c>
       <c r="F30">
         <f>SUM(F2:F27)</f>
-        <v>10.902200000000001</v>
+        <v>25.302199999999996</v>
       </c>
       <c r="H30">
         <f>SUM(H2:H27)</f>
@@ -957,8 +1048,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" tooltip="Add item to current order" display="http://www.mcmaster.com/nav/enter.asp?partnum=7489K12"/>
+    <hyperlink ref="B14" r:id="rId2" tooltip="Add item to current order" display="http://www.mcmaster.com/nav/enter.asp?partnum=7807K31"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>